<commit_message>
Deleted some error records
</commit_message>
<xml_diff>
--- a/2016SenatorsList.xlsx
+++ b/2016SenatorsList.xlsx
@@ -1,28 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramya/Documents/GitHub/Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bujji/Documents/MS_SMU/Capstone/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CC40AE-A5C2-A74B-B3C9-AA3FC62362E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$249</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$245</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="293">
   <si>
     <t>Republican</t>
   </si>
@@ -448,9 +444,6 @@
     <t>John Coyne</t>
   </si>
   <si>
-    <t>Allen Buckley</t>
-  </si>
-  <si>
     <t>Brian Schatz</t>
   </si>
   <si>
@@ -479,9 +472,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ray J. Writz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pro-Life </t>
   </si>
   <si>
     <t>Mark Kirk</t>
@@ -925,7 +915,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -989,18 +979,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1020,7 +1004,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1033,8 +1017,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1044,7 +1026,36 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1055,655 +1066,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Book1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Richard Shelby</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>Jonathan McConnell</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>John Martin</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Marcus Bowman</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>Shadrack McGill</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>Ron Crumpton</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>Charles Nana</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>Lisa Murkowski</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>Bob Lochner</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>Paul Kendall</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>Thomas Lamb</v>
-          </cell>
-          <cell r="L1" t="str">
-            <v>Ray Metcalfe</v>
-          </cell>
-          <cell r="M1" t="str">
-            <v>Edgar Blatchford</v>
-          </cell>
-          <cell r="N1" t="str">
-            <v>Cean Stevens</v>
-          </cell>
-          <cell r="O1" t="str">
-            <v>John McCain</v>
-          </cell>
-          <cell r="P1" t="str">
-            <v>Kelli Ward</v>
-          </cell>
-          <cell r="Q1" t="str">
-            <v>Alex Meluskey</v>
-          </cell>
-          <cell r="R1" t="str">
-            <v>Clair Van Steenwyk</v>
-          </cell>
-          <cell r="S1" t="str">
-            <v>Sean Webster</v>
-          </cell>
-          <cell r="T1" t="str">
-            <v>Ann Kirkpatrick</v>
-          </cell>
-          <cell r="U1" t="str">
-            <v>Alex Bello</v>
-          </cell>
-          <cell r="V1" t="str">
-            <v>Gary Swing</v>
-          </cell>
-          <cell r="W1" t="str">
-            <v>Merissa Hamilton</v>
-          </cell>
-          <cell r="X1" t="str">
-            <v>John Boozman</v>
-          </cell>
-          <cell r="Y1" t="str">
-            <v>Curtis Coleman</v>
-          </cell>
-          <cell r="Z1" t="str">
-            <v>Conner Eldridge</v>
-          </cell>
-          <cell r="AA1" t="str">
-            <v xml:space="preserve">Michael Bennet (Incumbent) </v>
-          </cell>
-          <cell r="AB1" t="str">
-            <v>Darryl Glenn</v>
-          </cell>
-          <cell r="AC1" t="str">
-            <v>Jack Graham</v>
-          </cell>
-          <cell r="AD1" t="str">
-            <v>Robert Blaha</v>
-          </cell>
-          <cell r="AE1" t="str">
-            <v>Jon Keyser</v>
-          </cell>
-          <cell r="AF1" t="str">
-            <v>Ryan Frazier</v>
-          </cell>
-          <cell r="AG1" t="str">
-            <v>Richard Blumenthal</v>
-          </cell>
-          <cell r="AH1" t="str">
-            <v>Dan Carter</v>
-          </cell>
-          <cell r="AI1" t="str">
-            <v>Richard Lion</v>
-          </cell>
-          <cell r="AJ1" t="str">
-            <v>Jeffery Russell</v>
-          </cell>
-          <cell r="AK1" t="str">
-            <v>Andrew Rule</v>
-          </cell>
-          <cell r="AL1" t="str">
-            <v xml:space="preserve">John M. Traceski </v>
-          </cell>
-          <cell r="AM1" t="str">
-            <v>Marco Rubio</v>
-          </cell>
-          <cell r="AN1" t="str">
-            <v>Carlos Beruff</v>
-          </cell>
-          <cell r="AO1" t="str">
-            <v>Dwight Young</v>
-          </cell>
-          <cell r="AP1" t="str">
-            <v>Ernie Rivera</v>
-          </cell>
-          <cell r="AQ1" t="str">
-            <v>Patrick Murphy</v>
-          </cell>
-          <cell r="AR1" t="str">
-            <v>Alan Grayson</v>
-          </cell>
-          <cell r="AS1" t="str">
-            <v>Pam Keith</v>
-          </cell>
-          <cell r="AT1" t="str">
-            <v xml:space="preserve">Rocky De La Fuente </v>
-          </cell>
-          <cell r="AU1" t="str">
-            <v>Reginald Luster</v>
-          </cell>
-          <cell r="AV1" t="str">
-            <v>Johnny Isakson</v>
-          </cell>
-          <cell r="AW1" t="str">
-            <v>Derrick Grayson</v>
-          </cell>
-          <cell r="AX1" t="str">
-            <v>Mary Kay</v>
-          </cell>
-          <cell r="AY1" t="str">
-            <v>Jim Barksdale</v>
-          </cell>
-          <cell r="AZ1" t="str">
-            <v>Cheryl Copeland</v>
-          </cell>
-          <cell r="BA1" t="str">
-            <v>John Coyne</v>
-          </cell>
-          <cell r="BB1" t="str">
-            <v>Johnny Isakson</v>
-          </cell>
-          <cell r="BC1" t="str">
-            <v>Jim Barksdale</v>
-          </cell>
-          <cell r="BD1" t="str">
-            <v>Allen Buckley</v>
-          </cell>
-          <cell r="BE1" t="str">
-            <v>Brian Schatz</v>
-          </cell>
-          <cell r="BF1" t="str">
-            <v>Makani Christensen</v>
-          </cell>
-          <cell r="BG1" t="str">
-            <v>Miles Shiratori</v>
-          </cell>
-          <cell r="BH1" t="str">
-            <v>Arturo Reyes</v>
-          </cell>
-          <cell r="BI1" t="str">
-            <v>Tutz Honeychurch</v>
-          </cell>
-          <cell r="BJ1" t="str">
-            <v>Joy Allison</v>
-          </cell>
-          <cell r="BK1" t="str">
-            <v>John Giuffre</v>
-          </cell>
-          <cell r="BL1" t="str">
-            <v>Mike Crapo</v>
-          </cell>
-          <cell r="BM1" t="str">
-            <v>Jerry Sturgill</v>
-          </cell>
-          <cell r="BN1" t="str">
-            <v xml:space="preserve">Ray J. Writz </v>
-          </cell>
-          <cell r="BO1" t="str">
-            <v xml:space="preserve">Pro-Life </v>
-          </cell>
-          <cell r="BP1" t="str">
-            <v>Mark Kirk</v>
-          </cell>
-          <cell r="BQ1" t="str">
-            <v>James T. Marter</v>
-          </cell>
-          <cell r="BR1" t="str">
-            <v>Tammy Duckworth</v>
-          </cell>
-          <cell r="BS1" t="str">
-            <v>Andrea Zopp</v>
-          </cell>
-          <cell r="BT1" t="str">
-            <v>Napoleon Harris</v>
-          </cell>
-          <cell r="BU1" t="str">
-            <v xml:space="preserve">Todd Young </v>
-          </cell>
-          <cell r="BV1" t="str">
-            <v xml:space="preserve">Marlin Stutzman </v>
-          </cell>
-          <cell r="BW1" t="str">
-            <v xml:space="preserve">Baron Hill </v>
-          </cell>
-          <cell r="BX1" t="str">
-            <v>Chuck Grassley</v>
-          </cell>
-          <cell r="BY1" t="str">
-            <v>Patty Judge</v>
-          </cell>
-          <cell r="BZ1" t="str">
-            <v>Rob Hogg</v>
-          </cell>
-          <cell r="CA1" t="str">
-            <v>Tom Fiegen</v>
-          </cell>
-          <cell r="CB1" t="str">
-            <v>Bob Krause</v>
-          </cell>
-          <cell r="CC1" t="str">
-            <v>Jerry Moran</v>
-          </cell>
-          <cell r="CD1" t="str">
-            <v>D.J. Smith</v>
-          </cell>
-          <cell r="CE1" t="str">
-            <v>Patrick Wiesner</v>
-          </cell>
-          <cell r="CF1" t="str">
-            <v>Monique Singh-Bey</v>
-          </cell>
-          <cell r="CG1" t="str">
-            <v>Rand Paul</v>
-          </cell>
-          <cell r="CH1" t="str">
-            <v>James Gould</v>
-          </cell>
-          <cell r="CI1" t="str">
-            <v>Stephen Slaughter</v>
-          </cell>
-          <cell r="CJ1" t="str">
-            <v>Jim Gray</v>
-          </cell>
-          <cell r="CK1" t="str">
-            <v>Sellus Wilder</v>
-          </cell>
-          <cell r="CL1" t="str">
-            <v>Ron Leach</v>
-          </cell>
-          <cell r="CM1" t="str">
-            <v>Tom Recktenwald</v>
-          </cell>
-          <cell r="CN1" t="str">
-            <v>Grant Short</v>
-          </cell>
-          <cell r="CO1" t="str">
-            <v>Jeff Kender</v>
-          </cell>
-          <cell r="CP1" t="str">
-            <v>Rory Houlihan</v>
-          </cell>
-          <cell r="CQ1" t="str">
-            <v>John Kennedy</v>
-          </cell>
-          <cell r="CR1" t="str">
-            <v>Foster Campbell</v>
-          </cell>
-          <cell r="CS1" t="str">
-            <v>Chris Van Hollen</v>
-          </cell>
-          <cell r="CT1" t="str">
-            <v>Donna Edwards</v>
-          </cell>
-          <cell r="CU1" t="str">
-            <v>Freddie Dickson</v>
-          </cell>
-          <cell r="CV1" t="str">
-            <v>Theresa Scaldaferri</v>
-          </cell>
-          <cell r="CW1" t="str">
-            <v>Violet Staley</v>
-          </cell>
-          <cell r="CX1" t="str">
-            <v>Lih Young</v>
-          </cell>
-          <cell r="CY1" t="str">
-            <v>Charles Smith</v>
-          </cell>
-          <cell r="CZ1" t="str">
-            <v>Ralph Jaffe</v>
-          </cell>
-          <cell r="DA1" t="str">
-            <v>Blaine Taylor</v>
-          </cell>
-          <cell r="DB1" t="str">
-            <v>Ed Tinus</v>
-          </cell>
-          <cell r="DC1" t="str">
-            <v>Kathy Szeliga</v>
-          </cell>
-          <cell r="DD1" t="str">
-            <v>Chris Chaffee</v>
-          </cell>
-          <cell r="DE1" t="str">
-            <v>Chrys Kefalas</v>
-          </cell>
-          <cell r="DF1" t="str">
-            <v>Richard Douglas</v>
-          </cell>
-          <cell r="DG1" t="str">
-            <v>Dave Wallace</v>
-          </cell>
-          <cell r="DH1" t="str">
-            <v>Sean Connor</v>
-          </cell>
-          <cell r="DI1" t="str">
-            <v>Lynn Richardson</v>
-          </cell>
-          <cell r="DJ1" t="str">
-            <v>John Graziani</v>
-          </cell>
-          <cell r="DK1" t="str">
-            <v>Greg Holmes</v>
-          </cell>
-          <cell r="DL1" t="str">
-            <v>Mark McNicholas</v>
-          </cell>
-          <cell r="DM1" t="str">
-            <v>Joe Hooe</v>
-          </cell>
-          <cell r="DN1" t="str">
-            <v>Anthony Seda</v>
-          </cell>
-          <cell r="DO1" t="str">
-            <v>Richard Shawver</v>
-          </cell>
-          <cell r="DP1" t="str">
-            <v>Garry Yarrington</v>
-          </cell>
-          <cell r="DQ1" t="str">
-            <v>Margaret Flowers</v>
-          </cell>
-          <cell r="DR1" t="str">
-            <v>Roy Blunt</v>
-          </cell>
-          <cell r="DS1" t="str">
-            <v>Kristi Nichols</v>
-          </cell>
-          <cell r="DT1" t="str">
-            <v>Ryan Luethy</v>
-          </cell>
-          <cell r="DU1" t="str">
-            <v>Bernie Mowinski</v>
-          </cell>
-          <cell r="DV1" t="str">
-            <v>Jason Kander</v>
-          </cell>
-          <cell r="DW1" t="str">
-            <v>Cori Bush</v>
-          </cell>
-          <cell r="DX1" t="str">
-            <v>Chief Wana Dubie</v>
-          </cell>
-          <cell r="DY1" t="str">
-            <v>Robert Mack</v>
-          </cell>
-          <cell r="DZ1" t="str">
-            <v>Jonathan Dine</v>
-          </cell>
-          <cell r="EA1" t="str">
-            <v>Herschel Young</v>
-          </cell>
-          <cell r="EB1" t="str">
-            <v>Fred Ryman</v>
-          </cell>
-          <cell r="EC1" t="str">
-            <v xml:space="preserve">Catherine Cortez Masto </v>
-          </cell>
-          <cell r="ED1" t="str">
-            <v xml:space="preserve">Allen Rheinhart </v>
-          </cell>
-          <cell r="EE1" t="str">
-            <v xml:space="preserve">Liddo Susan O'Briant </v>
-          </cell>
-          <cell r="EF1" t="str">
-            <v xml:space="preserve">Bobby Mahendra </v>
-          </cell>
-          <cell r="EG1" t="str">
-            <v>Joe Heck</v>
-          </cell>
-          <cell r="EH1" t="str">
-            <v>Sharron Angle</v>
-          </cell>
-          <cell r="EI1" t="str">
-            <v>Thomas Heck</v>
-          </cell>
-          <cell r="EJ1" t="str">
-            <v>Eddie Hamilton</v>
-          </cell>
-          <cell r="EK1" t="str">
-            <v>D'Nese Davis</v>
-          </cell>
-          <cell r="EL1" t="str">
-            <v>Bill Tarbell</v>
-          </cell>
-          <cell r="EM1" t="str">
-            <v>Robert Leeds</v>
-          </cell>
-          <cell r="EN1" t="str">
-            <v>Juston Preble</v>
-          </cell>
-          <cell r="EO1" t="str">
-            <v>Carlo Poliak</v>
-          </cell>
-          <cell r="EP1" t="str">
-            <v>Kelly Ayotte</v>
-          </cell>
-          <cell r="EQ1" t="str">
-            <v>Jim Rubens</v>
-          </cell>
-          <cell r="ER1" t="str">
-            <v>Tom Alciere</v>
-          </cell>
-          <cell r="ES1" t="str">
-            <v>Gerald Beloin</v>
-          </cell>
-          <cell r="ET1" t="str">
-            <v>Stanley Emanuel</v>
-          </cell>
-          <cell r="EU1" t="str">
-            <v>Maggie Hassan</v>
-          </cell>
-          <cell r="EV1" t="str">
-            <v>Chuck Schumer</v>
-          </cell>
-          <cell r="EW1" t="str">
-            <v>Wendy Long</v>
-          </cell>
-          <cell r="EX1" t="str">
-            <v>Robin Laverne Wilson</v>
-          </cell>
-          <cell r="EY1" t="str">
-            <v>Alex Merced</v>
-          </cell>
-          <cell r="EZ1" t="str">
-            <v>Richard Burr</v>
-          </cell>
-          <cell r="FA1" t="str">
-            <v>Greg Brannon</v>
-          </cell>
-          <cell r="FB1" t="str">
-            <v>Paul Wright</v>
-          </cell>
-          <cell r="FC1" t="str">
-            <v>Larry Holmquist</v>
-          </cell>
-          <cell r="FD1" t="str">
-            <v>Deborah Ross</v>
-          </cell>
-          <cell r="FE1" t="str">
-            <v>Chris Rey</v>
-          </cell>
-          <cell r="FF1" t="str">
-            <v>Kevin Griffin</v>
-          </cell>
-          <cell r="FG1" t="str">
-            <v>Ernest Reeves</v>
-          </cell>
-          <cell r="FH1" t="str">
-            <v>John Hoeven</v>
-          </cell>
-          <cell r="FI1" t="str">
-            <v>Eliot Glassheim</v>
-          </cell>
-          <cell r="FJ1" t="str">
-            <v>Robert Marquette</v>
-          </cell>
-          <cell r="FK1" t="str">
-            <v>Rob Portman</v>
-          </cell>
-          <cell r="FL1" t="str">
-            <v>Don Elijah Eckhart</v>
-          </cell>
-          <cell r="FM1" t="str">
-            <v>Ted Strickland</v>
-          </cell>
-          <cell r="FN1" t="str">
-            <v>P.G. Sittenfeld</v>
-          </cell>
-          <cell r="FO1" t="str">
-            <v>Kelli Prather</v>
-          </cell>
-          <cell r="FP1" t="str">
-            <v>Joe DeMare</v>
-          </cell>
-          <cell r="FQ1" t="str">
-            <v>Robert Murphy</v>
-          </cell>
-          <cell r="FR1" t="str">
-            <v>Dax Ewbank</v>
-          </cell>
-          <cell r="FS1" t="str">
-            <v>Ron Wyden</v>
-          </cell>
-          <cell r="FT1" t="str">
-            <v>Kevin Stine</v>
-          </cell>
-          <cell r="FU1" t="str">
-            <v>Paul Weaver</v>
-          </cell>
-          <cell r="FV1" t="str">
-            <v>Mark Callahan</v>
-          </cell>
-          <cell r="FW1" t="str">
-            <v>Sam Carpenter</v>
-          </cell>
-          <cell r="FX1" t="str">
-            <v>Faye Stewart</v>
-          </cell>
-          <cell r="FY1" t="str">
-            <v>Dan Laschober</v>
-          </cell>
-          <cell r="FZ1" t="str">
-            <v>Steven Reynolds</v>
-          </cell>
-          <cell r="GA1" t="str">
-            <v>Marvin Sandnes</v>
-          </cell>
-          <cell r="GB1" t="str">
-            <v>Pat Toomey</v>
-          </cell>
-          <cell r="GC1" t="str">
-            <v>Katie McGinty</v>
-          </cell>
-          <cell r="GD1" t="str">
-            <v>Joe Sestak</v>
-          </cell>
-          <cell r="GE1" t="str">
-            <v>John Fetterman</v>
-          </cell>
-          <cell r="GF1" t="str">
-            <v>Joseph Vodvarka</v>
-          </cell>
-          <cell r="GG1" t="str">
-            <v>Misty K. Snow</v>
-          </cell>
-          <cell r="GH1" t="str">
-            <v>Jonathan Swinton</v>
-          </cell>
-          <cell r="GI1" t="str">
-            <v>Patrick Leahy</v>
-          </cell>
-          <cell r="GJ1" t="str">
-            <v>Cris Ericson</v>
-          </cell>
-          <cell r="GK1" t="str">
-            <v>Patty Murray</v>
-          </cell>
-          <cell r="GL1" t="str">
-            <v>Chris Vance</v>
-          </cell>
-          <cell r="GM1" t="str">
-            <v>Eric John Markus</v>
-          </cell>
-          <cell r="GN1" t="str">
-            <v>Phil Cornell</v>
-          </cell>
-          <cell r="GO1" t="str">
-            <v>Scott Nazarino</v>
-          </cell>
-          <cell r="GP1" t="str">
-            <v>Mike Luke</v>
-          </cell>
-          <cell r="GQ1" t="str">
-            <v>Mohammad Said</v>
-          </cell>
-          <cell r="GR1" t="str">
-            <v>Donna Rae</v>
-          </cell>
-          <cell r="GS1" t="str">
-            <v>Ted Cummings</v>
-          </cell>
-          <cell r="GT1" t="str">
-            <v>Sam Wright</v>
-          </cell>
-          <cell r="GU1" t="str">
-            <v>Uncle Mover</v>
-          </cell>
-          <cell r="GV1" t="str">
-            <v>Jeremy Teuton</v>
-          </cell>
-          <cell r="GW1" t="str">
-            <v>Thor Amundson</v>
-          </cell>
-          <cell r="GX1" t="str">
-            <v>Chuck Jackson</v>
-          </cell>
-          <cell r="GY1" t="str">
-            <v>Pano Churchill</v>
-          </cell>
-          <cell r="GZ1" t="str">
-            <v>Zach Haller</v>
-          </cell>
-          <cell r="HA1" t="str">
-            <v>Alex Tsimerman</v>
-          </cell>
-          <cell r="HB1" t="str">
-            <v>Russ Feingold</v>
-          </cell>
-          <cell r="HC1" t="str">
-            <v>Scott Harbach</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1968,12 +1330,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D250"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="H245" sqref="H245"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2363,7 +1724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>4</v>
       </c>
@@ -2377,7 +1738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>4</v>
       </c>
@@ -2391,7 +1752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>0</v>
       </c>
@@ -2405,7 +1766,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +1780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>0</v>
       </c>
@@ -2433,7 +1794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +1808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>4</v>
       </c>
@@ -2461,7 +1822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>0</v>
       </c>
@@ -2475,7 +1836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +1850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>7</v>
       </c>
@@ -2503,7 +1864,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>4</v>
       </c>
@@ -2517,7 +1878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>8</v>
       </c>
@@ -2531,7 +1892,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>0</v>
       </c>
@@ -2545,7 +1906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>0</v>
       </c>
@@ -2559,7 +1920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>0</v>
       </c>
@@ -2573,9 +1934,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>88</v>
@@ -2587,7 +1948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>0</v>
       </c>
@@ -2601,7 +1962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>0</v>
       </c>
@@ -2615,7 +1976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>4</v>
       </c>
@@ -2629,7 +1990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>0</v>
       </c>
@@ -2643,7 +2004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>7</v>
       </c>
@@ -2657,7 +2018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>9</v>
       </c>
@@ -2671,9 +2032,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>95</v>
@@ -2685,7 +2046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>4</v>
       </c>
@@ -2699,7 +2060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>4</v>
       </c>
@@ -2713,9 +2074,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>98</v>
@@ -2727,9 +2088,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>99</v>
@@ -2741,9 +2102,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>100</v>
@@ -2755,9 +2116,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>101</v>
@@ -2769,9 +2130,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>102</v>
@@ -2783,9 +2144,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>103</v>
@@ -2797,9 +2158,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>104</v>
@@ -2811,9 +2172,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>105</v>
@@ -2825,9 +2186,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>106</v>
@@ -2839,7 +2200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>5</v>
       </c>
@@ -2853,7 +2214,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>5</v>
       </c>
@@ -2867,7 +2228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>5</v>
       </c>
@@ -3218,16 +2579,16 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B89" s="12" t="s">
+      <c r="A89" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C89" s="12">
+      <c r="C89" s="6">
         <v>166627</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D89" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3261,44 +2622,44 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C92" s="6">
-        <v>2135806</v>
+        <v>162891</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C93" s="12">
-        <v>1599726</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>24</v>
+      <c r="A93" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C93" s="6">
+        <v>11898</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C94" s="6">
-        <v>162260</v>
+        <v>8620</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -3306,10 +2667,10 @@
         <v>4</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C95" s="6">
-        <v>162891</v>
+        <v>3819</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>25</v>
@@ -3320,10 +2681,10 @@
         <v>4</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C96" s="6">
-        <v>11898</v>
+        <v>1815</v>
       </c>
       <c r="D96" s="10" t="s">
         <v>25</v>
@@ -3331,13 +2692,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C97" s="6">
-        <v>8620</v>
+        <v>217</v>
       </c>
       <c r="D97" s="10" t="s">
         <v>25</v>
@@ -3345,13 +2706,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C98" s="6">
-        <v>3819</v>
+        <v>111</v>
       </c>
       <c r="D98" s="10" t="s">
         <v>25</v>
@@ -3359,44 +2720,44 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C99" s="6">
-        <v>1815</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>25</v>
+        <v>119633</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C100" s="6">
-        <v>217</v>
-      </c>
-      <c r="D100" s="10" t="s">
-        <v>25</v>
+        <v>26471</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C101" s="6">
-        <v>111</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>25</v>
+        <v>131</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -3404,66 +2765,66 @@
         <v>0</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C102" s="6">
-        <v>119633</v>
+        <v>931619</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>146</v>
+        <v>287</v>
       </c>
       <c r="C103" s="6">
-        <v>26471</v>
+        <v>388571</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C104" s="6">
-        <v>131</v>
+        <v>1220128</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B105" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C105" s="12">
-        <v>89</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>26</v>
+      <c r="A105" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C105" s="6">
+        <v>455729</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C106" s="6">
-        <v>931619</v>
+        <v>219286</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>27</v>
@@ -3474,27 +2835,27 @@
         <v>0</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="C107" s="6">
-        <v>388571</v>
+        <v>151</v>
+      </c>
+      <c r="C107" s="7">
+        <v>661136</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
-        <v>4</v>
+        <v>292</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C108" s="6">
-        <v>1220128</v>
+        <v>152</v>
+      </c>
+      <c r="C108" s="7">
+        <v>324429</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -3502,55 +2863,55 @@
         <v>4</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C109" s="6">
-        <v>455729</v>
+        <v>153</v>
+      </c>
+      <c r="C109" s="8">
+        <v>516183</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C110" s="6">
-        <v>219286</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>27</v>
+        <v>90089</v>
+      </c>
+      <c r="D110" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C111" s="7">
-        <v>661136</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>18</v>
+        <v>155</v>
+      </c>
+      <c r="C111" s="6">
+        <v>46322</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C112" s="7">
-        <v>324429</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>18</v>
+        <v>156</v>
+      </c>
+      <c r="C112" s="6">
+        <v>37801</v>
+      </c>
+      <c r="D112" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -3558,24 +2919,24 @@
         <v>4</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C113" s="8">
-        <v>516183</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>18</v>
+        <v>157</v>
+      </c>
+      <c r="C113" s="6">
+        <v>6573</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C114" s="6">
-        <v>90089</v>
+        <v>6425</v>
       </c>
       <c r="D114" s="10" t="s">
         <v>28</v>
@@ -3583,30 +2944,30 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C115" s="6">
-        <v>46322</v>
-      </c>
-      <c r="D115" s="10" t="s">
-        <v>28</v>
+        <v>230907</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C116" s="6">
-        <v>37801</v>
-      </c>
-      <c r="D116" s="10" t="s">
-        <v>28</v>
+        <v>61056</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -3614,13 +2975,13 @@
         <v>4</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C117" s="6">
-        <v>6573</v>
-      </c>
-      <c r="D117" s="10" t="s">
-        <v>28</v>
+        <v>59522</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -3628,13 +2989,13 @@
         <v>4</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C118" s="6">
-        <v>6425</v>
-      </c>
-      <c r="D118" s="10" t="s">
-        <v>28</v>
+        <v>35042</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -3642,13 +3003,13 @@
         <v>0</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C119" s="6">
-        <v>230907</v>
+        <v>169180</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -3656,27 +3017,27 @@
         <v>0</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C120" s="6">
-        <v>61056</v>
+        <v>16611</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C121" s="6">
-        <v>59522</v>
+        <v>13728</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -3684,24 +3045,24 @@
         <v>4</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C122" s="6">
-        <v>35042</v>
+        <v>240613</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C123" s="6">
-        <v>169180</v>
+        <v>52728</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>30</v>
@@ -3709,13 +3070,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C124" s="6">
-        <v>16611</v>
+        <v>39026</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>30</v>
@@ -3723,13 +3084,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C125" s="6">
-        <v>13728</v>
+        <v>21910</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>30</v>
@@ -3740,10 +3101,10 @@
         <v>4</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C126" s="6">
-        <v>240613</v>
+        <v>21558</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>30</v>
@@ -3754,10 +3115,10 @@
         <v>4</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C127" s="6">
-        <v>52728</v>
+        <v>20239</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>30</v>
@@ -3768,10 +3129,10 @@
         <v>4</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C128" s="6">
-        <v>39026</v>
+        <v>13585</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>30</v>
@@ -3779,16 +3140,16 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C129" s="6">
-        <v>21910</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>30</v>
+        <v>536191</v>
+      </c>
+      <c r="D129" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -3796,13 +3157,13 @@
         <v>4</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C130" s="6">
-        <v>21558</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>30</v>
+        <v>347816</v>
+      </c>
+      <c r="D130" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -3810,13 +3171,13 @@
         <v>4</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C131" s="6">
-        <v>20239</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>30</v>
+        <v>470320</v>
+      </c>
+      <c r="D131" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -3824,27 +3185,27 @@
         <v>4</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C132" s="6">
-        <v>13585</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>30</v>
+        <v>343620</v>
+      </c>
+      <c r="D132" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C133" s="6">
-        <v>536191</v>
+        <v>14856</v>
       </c>
       <c r="D133" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -3852,13 +3213,13 @@
         <v>4</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C134" s="6">
-        <v>347816</v>
+        <v>13178</v>
       </c>
       <c r="D134" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -3866,10 +3227,10 @@
         <v>4</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C135" s="6">
-        <v>470320</v>
+        <v>10244</v>
       </c>
       <c r="D135" s="10" t="s">
         <v>32</v>
@@ -3880,10 +3241,10 @@
         <v>4</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C136" s="6">
-        <v>343620</v>
+        <v>8561</v>
       </c>
       <c r="D136" s="10" t="s">
         <v>32</v>
@@ -3894,10 +3255,10 @@
         <v>4</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C137" s="6">
-        <v>14856</v>
+        <v>7912</v>
       </c>
       <c r="D137" s="10" t="s">
         <v>32</v>
@@ -3908,10 +3269,10 @@
         <v>4</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C138" s="6">
-        <v>13178</v>
+        <v>7161</v>
       </c>
       <c r="D138" s="10" t="s">
         <v>32</v>
@@ -3922,10 +3283,10 @@
         <v>4</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C139" s="6">
-        <v>10244</v>
+        <v>5932</v>
       </c>
       <c r="D139" s="10" t="s">
         <v>32</v>
@@ -3936,10 +3297,10 @@
         <v>4</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C140" s="6">
-        <v>8561</v>
+        <v>2560</v>
       </c>
       <c r="D140" s="10" t="s">
         <v>32</v>
@@ -3947,13 +3308,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C141" s="6">
-        <v>7912</v>
+        <v>135337</v>
       </c>
       <c r="D141" s="10" t="s">
         <v>32</v>
@@ -3961,13 +3322,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C142" s="6">
-        <v>7161</v>
+        <v>52066</v>
       </c>
       <c r="D142" s="10" t="s">
         <v>32</v>
@@ -3975,13 +3336,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C143" s="6">
-        <v>5932</v>
+        <v>36340</v>
       </c>
       <c r="D143" s="10" t="s">
         <v>32</v>
@@ -3989,13 +3350,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C144" s="6">
-        <v>2560</v>
+        <v>29007</v>
       </c>
       <c r="D144" s="10" t="s">
         <v>32</v>
@@ -4006,10 +3367,10 @@
         <v>0</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C145" s="6">
-        <v>135337</v>
+        <v>23226</v>
       </c>
       <c r="D145" s="10" t="s">
         <v>32</v>
@@ -4020,10 +3381,10 @@
         <v>0</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C146" s="6">
-        <v>52066</v>
+        <v>21727</v>
       </c>
       <c r="D146" s="10" t="s">
         <v>32</v>
@@ -4034,10 +3395,10 @@
         <v>0</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C147" s="6">
-        <v>36340</v>
+        <v>20792</v>
       </c>
       <c r="D147" s="10" t="s">
         <v>32</v>
@@ -4048,10 +3409,10 @@
         <v>0</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C148" s="6">
-        <v>29007</v>
+        <v>16722</v>
       </c>
       <c r="D148" s="10" t="s">
         <v>32</v>
@@ -4062,10 +3423,10 @@
         <v>0</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C149" s="6">
-        <v>23226</v>
+        <v>16148</v>
       </c>
       <c r="D149" s="10" t="s">
         <v>32</v>
@@ -4076,10 +3437,10 @@
         <v>0</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C150" s="6">
-        <v>21727</v>
+        <v>9988</v>
       </c>
       <c r="D150" s="10" t="s">
         <v>32</v>
@@ -4090,10 +3451,10 @@
         <v>0</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C151" s="6">
-        <v>20792</v>
+        <v>8282</v>
       </c>
       <c r="D151" s="10" t="s">
         <v>32</v>
@@ -4104,10 +3465,10 @@
         <v>0</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C152" s="6">
-        <v>16722</v>
+        <v>3873</v>
       </c>
       <c r="D152" s="10" t="s">
         <v>32</v>
@@ -4118,10 +3479,10 @@
         <v>0</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C153" s="6">
-        <v>16148</v>
+        <v>3155</v>
       </c>
       <c r="D153" s="10" t="s">
         <v>32</v>
@@ -4132,10 +3493,10 @@
         <v>0</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C154" s="6">
-        <v>9988</v>
+        <v>2988</v>
       </c>
       <c r="D154" s="10" t="s">
         <v>32</v>
@@ -4143,13 +3504,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C155" s="6">
-        <v>8282</v>
+        <v>125</v>
       </c>
       <c r="D155" s="10" t="s">
         <v>32</v>
@@ -4160,13 +3521,13 @@
         <v>0</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C156" s="6">
-        <v>3873</v>
-      </c>
-      <c r="D156" s="10" t="s">
-        <v>32</v>
+        <v>481444</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -4174,13 +3535,13 @@
         <v>0</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C157" s="6">
-        <v>3155</v>
-      </c>
-      <c r="D157" s="10" t="s">
-        <v>32</v>
+        <v>134025</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -4188,38 +3549,38 @@
         <v>0</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C158" s="6">
-        <v>2988</v>
-      </c>
-      <c r="D158" s="10" t="s">
-        <v>32</v>
+        <v>29328</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C159" s="6">
-        <v>125</v>
-      </c>
-      <c r="D159" s="10" t="s">
-        <v>32</v>
+        <v>18789</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C160" s="6">
-        <v>481444</v>
+        <v>223492</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>19</v>
@@ -4227,13 +3588,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C161" s="6">
-        <v>134025</v>
+        <v>42453</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>19</v>
@@ -4241,13 +3602,13 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>204</v>
+        <v>288</v>
       </c>
       <c r="C162" s="6">
-        <v>29328</v>
+        <v>30432</v>
       </c>
       <c r="D162" s="6" t="s">
         <v>19</v>
@@ -4255,13 +3616,13 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C163" s="6">
-        <v>18789</v>
+        <v>23509</v>
       </c>
       <c r="D163" s="6" t="s">
         <v>19</v>
@@ -4269,13 +3630,13 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C164" s="6">
-        <v>223492</v>
+        <v>2002</v>
       </c>
       <c r="D164" s="6" t="s">
         <v>19</v>
@@ -4283,13 +3644,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C165" s="6">
-        <v>42453</v>
+        <v>1642</v>
       </c>
       <c r="D165" s="6" t="s">
         <v>19</v>
@@ -4297,125 +3658,125 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>290</v>
+        <v>209</v>
       </c>
       <c r="C166" s="6">
-        <v>30432</v>
+        <v>545</v>
       </c>
       <c r="D166" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C167" s="6">
-        <v>23509</v>
+        <v>210</v>
+      </c>
+      <c r="C167" s="5">
+        <v>81944</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C168" s="6">
-        <v>2002</v>
+        <v>211</v>
+      </c>
+      <c r="C168" s="5">
+        <v>5645</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C169" s="6">
-        <v>1642</v>
+        <v>212</v>
+      </c>
+      <c r="C169" s="5">
+        <v>4834</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C170" s="6">
-        <v>545</v>
+        <v>213</v>
+      </c>
+      <c r="C170" s="5">
+        <v>3760</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C171" s="5">
-        <v>81944</v>
+        <v>214</v>
+      </c>
+      <c r="C171" s="6">
+        <v>74517</v>
       </c>
       <c r="D171" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C172" s="5">
-        <v>5645</v>
+        <v>215</v>
+      </c>
+      <c r="C172" s="6">
+        <v>26142</v>
       </c>
       <c r="D172" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C173" s="5">
-        <v>4834</v>
+        <v>216</v>
+      </c>
+      <c r="C173" s="6">
+        <v>3570</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C174" s="5">
-        <v>3760</v>
+        <v>217</v>
+      </c>
+      <c r="C174" s="6">
+        <v>2507</v>
       </c>
       <c r="D174" s="6" t="s">
         <v>33</v>
@@ -4426,10 +3787,10 @@
         <v>0</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C175" s="6">
-        <v>74517</v>
+        <v>1937</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>33</v>
@@ -4440,10 +3801,10 @@
         <v>0</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C176" s="6">
-        <v>26142</v>
+        <v>1179</v>
       </c>
       <c r="D176" s="6" t="s">
         <v>33</v>
@@ -4454,10 +3815,10 @@
         <v>0</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C177" s="6">
-        <v>3570</v>
+        <v>662</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>33</v>
@@ -4468,10 +3829,10 @@
         <v>0</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C178" s="6">
-        <v>2507</v>
+        <v>582</v>
       </c>
       <c r="D178" s="6" t="s">
         <v>33</v>
@@ -4482,10 +3843,10 @@
         <v>0</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C179" s="6">
-        <v>1937</v>
+        <v>279</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>33</v>
@@ -4496,13 +3857,13 @@
         <v>0</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C180" s="6">
-        <v>1179</v>
+        <v>86558</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -4510,13 +3871,13 @@
         <v>0</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C181" s="6">
-        <v>662</v>
+        <v>19139</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -4524,13 +3885,13 @@
         <v>0</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C182" s="6">
-        <v>582</v>
+        <v>1586</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -4538,13 +3899,13 @@
         <v>0</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C183" s="6">
-        <v>279</v>
+        <v>1252</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -4552,10 +3913,10 @@
         <v>0</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C184" s="6">
-        <v>86558</v>
+        <v>1187</v>
       </c>
       <c r="D184" s="6" t="s">
         <v>34</v>
@@ -4563,13 +3924,13 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C185" s="6">
-        <v>19139</v>
+        <v>301</v>
       </c>
       <c r="D185" s="6" t="s">
         <v>34</v>
@@ -4577,125 +3938,125 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C186" s="6">
-        <v>1586</v>
+        <v>5221945</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C187" s="6">
-        <v>1252</v>
+        <v>2009335</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="6" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>229</v>
+        <v>289</v>
       </c>
       <c r="C188" s="6">
-        <v>1187</v>
+        <v>13413</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C189" s="6">
-        <v>301</v>
+        <v>48120</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C190" s="6">
-        <v>5221945</v>
+        <v>622074</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C191" s="6">
-        <v>2009335</v>
+        <v>255030</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="6" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>291</v>
+        <v>234</v>
       </c>
       <c r="C192" s="6">
-        <v>13413</v>
+        <v>85944</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C193" s="6">
-        <v>48120</v>
+        <v>50010</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C194" s="6">
-        <v>622074</v>
+        <v>614414</v>
       </c>
       <c r="D194" s="6" t="s">
         <v>36</v>
@@ -4703,13 +4064,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C195" s="6">
-        <v>255030</v>
+        <v>162869</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>36</v>
@@ -4717,13 +4078,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C196" s="6">
-        <v>85944</v>
+        <v>115618</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>36</v>
@@ -4731,13 +4092,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C197" s="6">
-        <v>50010</v>
+        <v>93005</v>
       </c>
       <c r="D197" s="6" t="s">
         <v>36</v>
@@ -4745,58 +4106,58 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C198" s="6">
-        <v>614414</v>
+        <v>103677</v>
       </c>
       <c r="D198" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C199" s="6">
-        <v>162869</v>
+        <v>17243</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C200" s="6">
-        <v>115618</v>
-      </c>
-      <c r="D200" s="6" t="s">
-        <v>36</v>
+        <v>1089</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C201" s="6">
-        <v>93005</v>
+        <v>1336686</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -4804,52 +4165,52 @@
         <v>0</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>242</v>
+        <v>290</v>
       </c>
       <c r="C202" s="6">
-        <v>103677</v>
+        <v>290268</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C203" s="6">
-        <v>17243</v>
+        <v>742676</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C204" s="6">
-        <v>1089</v>
-      </c>
-      <c r="D204" s="1" t="s">
-        <v>37</v>
+        <v>254232</v>
+      </c>
+      <c r="D204" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C205" s="6">
-        <v>1336686</v>
+        <v>144945</v>
       </c>
       <c r="D205" s="6" t="s">
         <v>38</v>
@@ -4857,13 +4218,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="6" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>292</v>
+        <v>247</v>
       </c>
       <c r="C206" s="6">
-        <v>290268</v>
+        <v>3123</v>
       </c>
       <c r="D206" s="6" t="s">
         <v>38</v>
@@ -4871,30 +4232,30 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C207" s="6">
-        <v>742676</v>
+        <v>1537</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C208" s="6">
-        <v>254232</v>
+        <v>1073</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
@@ -4902,66 +4263,66 @@
         <v>4</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C209" s="6">
-        <v>144945</v>
+        <v>501903</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C210" s="6">
-        <v>3123</v>
+        <v>78287</v>
       </c>
       <c r="D210" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C211" s="6">
-        <v>1537</v>
+        <v>20346</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C212" s="6">
-        <v>1073</v>
+        <v>123473</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C213" s="6">
-        <v>501903</v>
+        <v>104494</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>40</v>
@@ -4969,13 +4330,13 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C214" s="6">
-        <v>78287</v>
+        <v>57399</v>
       </c>
       <c r="D214" s="6" t="s">
         <v>40</v>
@@ -4983,13 +4344,13 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C215" s="6">
-        <v>20346</v>
+        <v>34157</v>
       </c>
       <c r="D215" s="6" t="s">
         <v>40</v>
@@ -4997,13 +4358,13 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C216" s="6">
-        <v>123473</v>
+        <v>10497</v>
       </c>
       <c r="D216" s="6" t="s">
         <v>40</v>
@@ -5011,13 +4372,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C217" s="6">
-        <v>104494</v>
+        <v>4733</v>
       </c>
       <c r="D217" s="6" t="s">
         <v>40</v>
@@ -5028,66 +4389,66 @@
         <v>0</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C218" s="6">
-        <v>57399</v>
+        <v>1342941</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C219" s="6">
-        <v>34157</v>
+        <v>669774</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C220" s="6">
-        <v>10497</v>
+        <v>513221</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C221" s="6">
-        <v>4733</v>
+        <v>307090</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C222" s="6">
-        <v>1342941</v>
+        <v>85837</v>
       </c>
       <c r="D222" s="6" t="s">
         <v>41</v>
@@ -5098,13 +4459,13 @@
         <v>4</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C223" s="6">
-        <v>669774</v>
-      </c>
-      <c r="D223" s="6" t="s">
-        <v>41</v>
+        <v>28928</v>
+      </c>
+      <c r="D223" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -5112,13 +4473,13 @@
         <v>4</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C224" s="6">
-        <v>513221</v>
-      </c>
-      <c r="D224" s="6" t="s">
-        <v>41</v>
+        <v>19774</v>
+      </c>
+      <c r="D224" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -5126,13 +4487,13 @@
         <v>4</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C225" s="6">
-        <v>307090</v>
-      </c>
-      <c r="D225" s="6" t="s">
-        <v>41</v>
+        <v>192243</v>
+      </c>
+      <c r="D225" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -5140,13 +4501,13 @@
         <v>4</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C226" s="6">
-        <v>85837</v>
-      </c>
-      <c r="D226" s="6" t="s">
-        <v>41</v>
+        <v>7595</v>
+      </c>
+      <c r="D226" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -5154,41 +4515,41 @@
         <v>4</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C227" s="6">
-        <v>28928</v>
+        <v>745421</v>
       </c>
       <c r="D227" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C228" s="6">
-        <v>19774</v>
+        <v>269</v>
+      </c>
+      <c r="C228" s="11">
+        <v>381004</v>
       </c>
       <c r="D228" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C229" s="6">
-        <v>192243</v>
+        <v>57825</v>
       </c>
       <c r="D229" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -5196,24 +4557,24 @@
         <v>4</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C230" s="6">
-        <v>7595</v>
+        <v>46460</v>
       </c>
       <c r="D230" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C231" s="6">
-        <v>745421</v>
+        <v>41542</v>
       </c>
       <c r="D231" s="10" t="s">
         <v>44</v>
@@ -5221,13 +4582,13 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C232" s="11">
-        <v>381004</v>
+        <v>273</v>
+      </c>
+      <c r="C232" s="6">
+        <v>20988</v>
       </c>
       <c r="D232" s="10" t="s">
         <v>44</v>
@@ -5235,13 +4596,13 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C233" s="6">
-        <v>57825</v>
+        <v>13362</v>
       </c>
       <c r="D233" s="10" t="s">
         <v>44</v>
@@ -5249,13 +4610,13 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C234" s="6">
-        <v>46460</v>
+        <v>11472</v>
       </c>
       <c r="D234" s="10" t="s">
         <v>44</v>
@@ -5263,13 +4624,13 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C235" s="6">
-        <v>41542</v>
+        <v>11028</v>
       </c>
       <c r="D235" s="10" t="s">
         <v>44</v>
@@ -5277,13 +4638,13 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B236" s="6" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C236" s="6">
-        <v>20988</v>
+        <v>10751</v>
       </c>
       <c r="D236" s="10" t="s">
         <v>44</v>
@@ -5291,13 +4652,13 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C237" s="6">
-        <v>13362</v>
+        <v>8569</v>
       </c>
       <c r="D237" s="10" t="s">
         <v>44</v>
@@ -5308,10 +4669,10 @@
         <v>6</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C238" s="6">
-        <v>11472</v>
+        <v>7991</v>
       </c>
       <c r="D238" s="10" t="s">
         <v>44</v>
@@ -5319,13 +4680,13 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C239" s="6">
-        <v>11028</v>
+        <v>7906</v>
       </c>
       <c r="D239" s="10" t="s">
         <v>44</v>
@@ -5336,10 +4697,10 @@
         <v>6</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C240" s="6">
-        <v>10751</v>
+        <v>6318</v>
       </c>
       <c r="D240" s="10" t="s">
         <v>44</v>
@@ -5347,13 +4708,13 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="6" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C241" s="6">
-        <v>8569</v>
+        <v>5150</v>
       </c>
       <c r="D241" s="10" t="s">
         <v>44</v>
@@ -5364,10 +4725,10 @@
         <v>6</v>
       </c>
       <c r="B242" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C242" s="6">
-        <v>7991</v>
+        <v>5092</v>
       </c>
       <c r="D242" s="10" t="s">
         <v>44</v>
@@ -5375,13 +4736,13 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B243" s="6" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C243" s="6">
-        <v>7906</v>
+        <v>4117</v>
       </c>
       <c r="D243" s="10" t="s">
         <v>44</v>
@@ -5389,138 +4750,48 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B244" s="6" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C244" s="6">
-        <v>6318</v>
+        <v>303282</v>
       </c>
       <c r="D244" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C245" s="6">
-        <v>5150</v>
+        <v>33185</v>
       </c>
       <c r="D245" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A246" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B246" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="C246" s="6">
-        <v>5092</v>
-      </c>
-      <c r="D246" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A247" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B247" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C247" s="6">
-        <v>4117</v>
-      </c>
-      <c r="D247" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A248" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B248" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C248" s="6">
-        <v>303282</v>
-      </c>
-      <c r="D248" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A249" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B249" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="C249" s="6">
-        <v>33185</v>
-      </c>
-      <c r="D249" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A250" s="9"/>
-      <c r="B250" s="9"/>
-      <c r="C250" s="9"/>
-      <c r="D250" s="9"/>
+    <row r="246" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="9"/>
+      <c r="B246" s="9"/>
+      <c r="C246" s="9"/>
+      <c r="D246" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D249" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Alabama"/>
-        <filter val="Alaska"/>
-        <filter val="Arizona"/>
-        <filter val="Arkansas"/>
-        <filter val="Colorado"/>
-        <filter val="Connecticut"/>
-        <filter val="Florida"/>
-        <filter val="Georgia"/>
-        <filter val="Hawaii"/>
-        <filter val="Idaho"/>
-        <filter val="Illinois"/>
-        <filter val="Indiana"/>
-        <filter val="Iowa"/>
-        <filter val="Kansas"/>
-        <filter val="Kentucky"/>
-        <filter val="Louisiana"/>
-        <filter val="Maryland"/>
-        <filter val="Missouri"/>
-        <filter val="Nevada"/>
-        <filter val="New Hampshire"/>
-        <filter val="New York"/>
-        <filter val="North Carolina"/>
-        <filter val="North Dakota"/>
-        <filter val="Ohio"/>
-        <filter val="Oklahoma"/>
-        <filter val="Oregon"/>
-        <filter val="Pennsylvania"/>
-        <filter val="Utah"/>
-        <filter val="Vermont"/>
-        <filter val="Washington"/>
-        <filter val="Wisconsin"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C24F5C-BA93-F94D-B14E-F66632C95748}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>